<commit_message>
update - analisi di dispersione
</commit_message>
<xml_diff>
--- a/Analisi Univariata/Analisi Monovariata.xlsx
+++ b/Analisi Univariata/Analisi Monovariata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carmi\Desktop\Unisa Magistrale\SAD\Progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carmi\Desktop\Unisa Magistrale\SAD\SAD_Alcol_Consume_Italy_2019\Analisi Univariata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB70F0F2-A296-4464-A67D-3A9363BC491F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B6ABA8-5F5C-4DD0-907C-BB0D5D89AA71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EA12E6F-9D00-4C5C-A91F-481F1E6401BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve"> Piemonte</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Regioni</t>
+  </si>
+  <si>
+    <t>Scarto dalla media</t>
+  </si>
+  <si>
+    <t>Nuovo Valore Ideale</t>
+  </si>
+  <si>
+    <t>Vettore Ideale</t>
   </si>
 </sst>
 </file>
@@ -115,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,14 +150,29 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="7"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,18 +181,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,11 +227,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -206,20 +253,34 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -539,7 +600,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E2" sqref="E2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,238 +608,399 @@
     <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="C1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="9">
         <v>16</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="C2" s="9">
+        <f xml:space="preserve"> B2 - 182.4</f>
+        <v>-166.4</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>25</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:E23" si="0" xml:space="preserve"> B3 - 182.4</f>
+        <v>-157.4</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>41</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="C4" s="9">
+        <f t="shared" si="0"/>
+        <v>-141.4</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="9">
         <v>53</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="9">
+        <f t="shared" si="0"/>
+        <v>-129.4</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="10">
         <v>56</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>-126.4</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="10">
         <v>73</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>-109.4</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="10">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="9">
         <v>83</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>-99.4</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="9">
         <v>96</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>-86.4</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="9">
         <v>110</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>-72.400000000000006</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="9">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="9">
         <v>110</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>-72.400000000000006</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="9">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="9">
         <v>122</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>-60.400000000000006</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="9">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="9">
         <v>129</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>-53.400000000000006</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="9">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="9">
         <v>167</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>-15.400000000000006</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="9">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>197</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>14.599999999999994</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="7">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>197</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>14.599999999999994</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="7">
+        <v>197</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>211</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>28.599999999999994</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="7">
+        <v>211</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>223</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>40.599999999999994</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="7">
+        <v>223</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="5">
         <v>310</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="12">
+        <f t="shared" si="0"/>
+        <v>127.6</v>
+      </c>
+      <c r="D19" s="9">
+        <f>B19-C19</f>
+        <v>182.4</v>
+      </c>
+      <c r="E19" s="9">
+        <f>D19</f>
+        <v>182.4</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="5">
         <v>311</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="12">
+        <f t="shared" si="0"/>
+        <v>128.6</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" ref="D20:E23" si="1">B20-C20</f>
+        <v>182.4</v>
+      </c>
+      <c r="E20" s="9">
+        <f t="shared" ref="E20:E23" si="2">D20</f>
+        <v>182.4</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="5">
         <v>316</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="C21" s="12">
+        <f t="shared" si="0"/>
+        <v>133.6</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="1"/>
+        <v>182.4</v>
+      </c>
+      <c r="E21" s="9">
+        <f t="shared" si="2"/>
+        <v>182.4</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="5">
         <v>394</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="12">
+        <f t="shared" si="0"/>
+        <v>211.6</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="1"/>
+        <v>182.4</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" si="2"/>
+        <v>182.4</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="5">
         <v>719</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="12">
+        <f t="shared" si="0"/>
+        <v>536.6</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="1"/>
+        <v>182.39999999999998</v>
+      </c>
+      <c r="E23" s="9">
+        <f t="shared" si="2"/>
+        <v>182.39999999999998</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>

</xml_diff>